<commit_message>
Try to find the way to avoid obstacles
</commit_message>
<xml_diff>
--- a/Liens - article - etc/Lien utiles.xlsx
+++ b/Liens - article - etc/Lien utiles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darkz\Desktop\TIPE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darkz\Desktop\TIPE\Liens - article - etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B432E8BD-E0AF-4641-95FD-42C4BB1020DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D0D8CB-CC43-49B9-AD6E-82DA32216826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
   <si>
     <t>https://citeseerx.ist.psu.edu/viewdoc/download?doi=10.1.1.611.1374&amp;rep=rep1&amp;type=pdf</t>
   </si>
@@ -178,6 +178,45 @@
   </si>
   <si>
     <t>https://jhttps://reader.elsevier.com/reader/sd/pii/S2352146514001215?token=6F99D6528487008D47035AF24FC5A0281CEC010618001CC6FF1ECAA1D3EC342E2DD52A05CFDB49602D8B45C30FB2D4B1&amp;originRegion=eu-west-1&amp;originCreation=20220217162511</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ieeexplore.ieee.org/abstract/document/488968 </t>
+  </si>
+  <si>
+    <t>PSO: James Kennedy</t>
+  </si>
+  <si>
+    <t>Algorithme PSO</t>
+  </si>
+  <si>
+    <t>https://tel.archives-ouvertes.fr/tel-00523176/</t>
+  </si>
+  <si>
+    <t>Thèse</t>
+  </si>
+  <si>
+    <t>Modélisation du mouvement des personnes lors de l’évacuation d’un bâtiment à la suite d’un sinistre</t>
+  </si>
+  <si>
+    <t>https://indico.ijclab.in2p3.fr/event/2382/contributions/4592/attachments/4351/5296/Bertrand_Maury.pdf</t>
+  </si>
+  <si>
+    <t>Simulation de mouvements de foules</t>
+  </si>
+  <si>
+    <t>Space-time Simulation Model Based on Particle Swarm Optimization Algorithm for Stadium Evacuation</t>
+  </si>
+  <si>
+    <t>https://ir.nsfc.gov.cn//paperDownload/1000008859916.pdf</t>
+  </si>
+  <si>
+    <t>Swarm Intelligence in Evacuation Problems: a Review</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/300546019_Swarm_Intelligence_in_Evacuation_Problems_A_Review</t>
+  </si>
+  <si>
+    <t>https://complex-systems-ai.com/algorithmes-dessaims/ ou https://complex-systems-ai.com/en/algorithms-desaims/particle-swarm/</t>
   </si>
 </sst>
 </file>
@@ -567,16 +606,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="140.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="143.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="255.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -825,6 +864,72 @@
       </c>
       <c r="C23" s="1" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -843,8 +948,14 @@
     <hyperlink ref="C21" r:id="rId11" xr:uid="{C69C837A-23DA-4F52-A4FC-A64BF8FB3924}"/>
     <hyperlink ref="C13" r:id="rId12" xr:uid="{577C664F-3A99-4643-B3F9-57610ADA5D10}"/>
     <hyperlink ref="C14" r:id="rId13" xr:uid="{EF99EE35-B87B-48AE-BD2E-3DD5E452F044}"/>
+    <hyperlink ref="C24" r:id="rId14" display="https://ieeexplore.ieee.org/abstract/document/488968" xr:uid="{30104839-F55A-4D6C-A9FE-25E11D119490}"/>
+    <hyperlink ref="C29" r:id="rId15" xr:uid="{AB780877-1D39-4440-B966-D8D31DF43888}"/>
+    <hyperlink ref="C28" r:id="rId16" xr:uid="{34460C71-E9DB-46AC-998D-98CB4C7F5F79}"/>
+    <hyperlink ref="C27" r:id="rId17" xr:uid="{B0A410FE-2409-4B43-96F7-3DDAC8A100C5}"/>
+    <hyperlink ref="C26" r:id="rId18" xr:uid="{E5D6128C-B0C8-42A0-8213-B4DC421FC1E0}"/>
+    <hyperlink ref="C25" r:id="rId19" display="https://complex-systems-ai.com/algorithmes-dessaims/" xr:uid="{BEAB7A3A-CCB1-4CB6-9EEE-9ABFF98E49B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>